<commit_message>
99IOS TCs second push 06.05.2025
</commit_message>
<xml_diff>
--- a/Data Files/Excel_Files/Validation_Messages.xlsx
+++ b/Data Files/Excel_Files/Validation_Messages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52376032\Katalon Studio\Mytix_IOS\Data Files\Excel_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52376032\Katalon Studio\Mytix_IOS_Katalon_Sripts\Data Files\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFE1AD7-EEF6-451D-B372-9CE8D258CBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAC18D1-DFB6-4065-BEA4-636213085648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="380" windowWidth="19180" windowHeight="10180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Message_ID</t>
   </si>
@@ -89,6 +89,11 @@
   </si>
   <si>
     <t>Invalid User Id/Password.</t>
+  </si>
+  <si>
+    <t>The NJ TRANSIT portion of this joint ticket will expire 30 days from the date of purchase.
+The SEPTA portion of this joint ticket will expire 180 days from the date of purchase.
+Tickets are valid in either direction.</t>
   </si>
 </sst>
 </file>
@@ -124,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -134,6 +139,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -415,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -548,6 +556,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="16" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>